<commit_message>
Make TSP2 ready to branch and bound
</commit_message>
<xml_diff>
--- a/Input Data2.xlsx
+++ b/Input Data2.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KMITL\Year2 1st\Linear Algebra\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FC5D2D3-1B0E-4817-ADB9-5F5B1FAC63C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E9784C-C328-440E-9654-2391149E9D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="810" windowWidth="21600" windowHeight="13755" xr2:uid="{1DE7C1F6-1C4D-4A62-9771-A330E52E4FA7}"/>
+    <workbookView xWindow="1020" yWindow="1065" windowWidth="21600" windowHeight="13755" xr2:uid="{1DE7C1F6-1C4D-4A62-9771-A330E52E4FA7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Car" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,24 +35,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>1,2,3,4</t>
-  </si>
-  <si>
-    <t>2,3,4,5</t>
-  </si>
-  <si>
-    <t>0,2,3,5</t>
-  </si>
-  <si>
-    <t>2,2,3,5</t>
-  </si>
-  <si>
-    <t>1,2,5,6</t>
-  </si>
-  <si>
-    <t>0,4,5,6</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>b,3,0,0</t>
+  </si>
+  <si>
+    <t>c,7,0,0</t>
+  </si>
+  <si>
+    <t>a,3,0,0</t>
+  </si>
+  <si>
+    <t>d,5,0,0</t>
+  </si>
+  <si>
+    <t>a,7,0,0</t>
+  </si>
+  <si>
+    <t>d,9,0,0</t>
+  </si>
+  <si>
+    <t>b,5,0,0</t>
+  </si>
+  <si>
+    <t>c,9,0,0</t>
+  </si>
+  <si>
+    <t>e,2,0,0</t>
+  </si>
+  <si>
+    <t>f,1,0,0</t>
+  </si>
+  <si>
+    <t>d,2,0,0</t>
+  </si>
+  <si>
+    <t>g,3,0,0</t>
+  </si>
+  <si>
+    <t>d,1,0,0</t>
+  </si>
+  <si>
+    <t>g,4,0,0</t>
+  </si>
+  <si>
+    <t>e,3,0,0</t>
+  </si>
+  <si>
+    <t>f,4,0,0</t>
   </si>
 </sst>
 </file>
@@ -96,8 +147,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="ปกติ" xfId="0" builtinId="0"/>
@@ -412,46 +466,108 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FD3B8F-FF11-493D-A750-C76D2FC337AD}">
-  <dimension ref="A2:C4"/>
+  <dimension ref="A2:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Ready to use try dp
</commit_message>
<xml_diff>
--- a/Input Data2.xlsx
+++ b/Input Data2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KMITL\Year2 1st\Linear Algebra\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E9784C-C328-440E-9654-2391149E9D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81637A85-C6FB-4BFA-8BA1-8F6CD5D7596E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="1065" windowWidth="21600" windowHeight="13755" xr2:uid="{1DE7C1F6-1C4D-4A62-9771-A330E52E4FA7}"/>
   </bookViews>
@@ -469,7 +469,7 @@
   <dimension ref="A2:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
TSP update(can visit node more than once)
</commit_message>
<xml_diff>
--- a/Input Data2.xlsx
+++ b/Input Data2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KMITL\Year2 1st\Linear Algebra\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81637A85-C6FB-4BFA-8BA1-8F6CD5D7596E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7865D60-7B2A-4CC0-9B50-C4A4F11B5613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1020" yWindow="1065" windowWidth="21600" windowHeight="13755" xr2:uid="{1DE7C1F6-1C4D-4A62-9771-A330E52E4FA7}"/>
   </bookViews>
@@ -55,46 +55,46 @@
     <t>f</t>
   </si>
   <si>
+    <t>b,3,0,0</t>
+  </si>
+  <si>
+    <t>c,7,0,0</t>
+  </si>
+  <si>
+    <t>a,3,0,0</t>
+  </si>
+  <si>
+    <t>d,5,0,0</t>
+  </si>
+  <si>
+    <t>a,7,0,0</t>
+  </si>
+  <si>
+    <t>d,9,0,0</t>
+  </si>
+  <si>
+    <t>b,5,0,0</t>
+  </si>
+  <si>
+    <t>c,9,0,0</t>
+  </si>
+  <si>
+    <t>e,2,0,0</t>
+  </si>
+  <si>
+    <t>f,1,0,0</t>
+  </si>
+  <si>
+    <t>d,2,0,0</t>
+  </si>
+  <si>
+    <t>d,1,0,0</t>
+  </si>
+  <si>
     <t>g</t>
   </si>
   <si>
-    <t>b,3,0,0</t>
-  </si>
-  <si>
-    <t>c,7,0,0</t>
-  </si>
-  <si>
-    <t>a,3,0,0</t>
-  </si>
-  <si>
-    <t>d,5,0,0</t>
-  </si>
-  <si>
-    <t>a,7,0,0</t>
-  </si>
-  <si>
-    <t>d,9,0,0</t>
-  </si>
-  <si>
-    <t>b,5,0,0</t>
-  </si>
-  <si>
-    <t>c,9,0,0</t>
-  </si>
-  <si>
-    <t>e,2,0,0</t>
-  </si>
-  <si>
-    <t>f,1,0,0</t>
-  </si>
-  <si>
-    <t>d,2,0,0</t>
-  </si>
-  <si>
     <t>g,3,0,0</t>
-  </si>
-  <si>
-    <t>d,1,0,0</t>
   </si>
   <si>
     <t>g,4,0,0</t>
@@ -469,7 +469,7 @@
   <dimension ref="A2:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -479,10 +479,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
@@ -492,10 +492,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -505,10 +505,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -518,16 +518,16 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -535,10 +535,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -548,7 +548,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>20</v>
@@ -558,7 +558,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Finished TSP and combination
</commit_message>
<xml_diff>
--- a/Input Data2.xlsx
+++ b/Input Data2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KMITL\Year2 1st\Linear Algebra\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7865D60-7B2A-4CC0-9B50-C4A4F11B5613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F830676-2D8B-42CB-B28B-3ABD17FAC909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="1065" windowWidth="21600" windowHeight="13755" xr2:uid="{1DE7C1F6-1C4D-4A62-9771-A330E52E4FA7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1DE7C1F6-1C4D-4A62-9771-A330E52E4FA7}"/>
   </bookViews>
   <sheets>
     <sheet name="Car" sheetId="1" r:id="rId1"/>
@@ -35,75 +35,93 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>e</t>
-  </si>
-  <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>b,3,0,0</t>
-  </si>
-  <si>
-    <t>c,7,0,0</t>
-  </si>
-  <si>
-    <t>a,3,0,0</t>
-  </si>
-  <si>
-    <t>d,5,0,0</t>
-  </si>
-  <si>
-    <t>a,7,0,0</t>
-  </si>
-  <si>
-    <t>d,9,0,0</t>
-  </si>
-  <si>
-    <t>b,5,0,0</t>
-  </si>
-  <si>
-    <t>c,9,0,0</t>
-  </si>
-  <si>
-    <t>e,2,0,0</t>
-  </si>
-  <si>
-    <t>f,1,0,0</t>
-  </si>
-  <si>
-    <t>d,2,0,0</t>
-  </si>
-  <si>
-    <t>d,1,0,0</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>g,3,0,0</t>
-  </si>
-  <si>
-    <t>g,4,0,0</t>
-  </si>
-  <si>
-    <t>e,3,0,0</t>
-  </si>
-  <si>
-    <t>f,4,0,0</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+  <si>
+    <t>IcecreamShop,0.5,5,0</t>
+  </si>
+  <si>
+    <t>Subway St.1,3,10,5</t>
+  </si>
+  <si>
+    <t>Subway St.1</t>
+  </si>
+  <si>
+    <t>Subway St.2,25,35,15</t>
+  </si>
+  <si>
+    <t>Subway St.3,15,20,10</t>
+  </si>
+  <si>
+    <t>Subway St.2</t>
+  </si>
+  <si>
+    <t>mall,0.3,5,0</t>
+  </si>
+  <si>
+    <t>Start,3,10,5</t>
+  </si>
+  <si>
+    <t>Subway St.1,25,35,15</t>
+  </si>
+  <si>
+    <t>Subway St.1,15,20,10</t>
+  </si>
+  <si>
+    <t>Cafe,5,10,10</t>
+  </si>
+  <si>
+    <t>Aquarium,3,7,5</t>
+  </si>
+  <si>
+    <t>GameCenter,8,10,20</t>
+  </si>
+  <si>
+    <t>Subway St.3</t>
+  </si>
+  <si>
+    <t>Subway St.3,5,10,10</t>
+  </si>
+  <si>
+    <t>Cafe</t>
+  </si>
+  <si>
+    <t>Aquarium</t>
+  </si>
+  <si>
+    <t>Aquarium,1000,120,20000</t>
+  </si>
+  <si>
+    <t>Cafe,1000,120,20000</t>
+  </si>
+  <si>
+    <t>Subway St.3,3,7,5</t>
+  </si>
+  <si>
+    <t>GameCenter,4,5,2</t>
+  </si>
+  <si>
+    <t>GameCenter</t>
+  </si>
+  <si>
+    <t>Aquarium,4,5,2</t>
+  </si>
+  <si>
+    <t>Subway St.3,8,10,20</t>
+  </si>
+  <si>
+    <t>IcecreamShop</t>
+  </si>
+  <si>
+    <t>Start,0.5,5,0</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>mall</t>
+  </si>
+  <si>
+    <t>Subway St.2,0.3,5,0</t>
   </si>
 </sst>
 </file>
@@ -466,108 +484,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8FD3B8F-FF11-493D-A750-C76D2FC337AD}">
-  <dimension ref="A2:E8"/>
+  <dimension ref="A2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="11" width="34.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="1"/>
+        <v>4</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="1"/>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>